<commit_message>
Update link-prospect-relevance and similarity_matrix CSV files with new loan-related keywords and their cosine similarities; remove obsolete keyword-internal-link mapping Excel file.
</commit_message>
<xml_diff>
--- a/scripts/keyword-internal-link-mapping.xlsx
+++ b/scripts/keyword-internal-link-mapping.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C67"/>
+  <dimension ref="A1:C89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,1122 +453,1496 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>nmims mba</t>
+          <t>personal loans</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://sbm.nmims.edu/mba-program</t>
+          <t>https://www.tatacapital.com/personal-loan.html</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/fulltime-programs', 'https://sbm.nmims.edu/mba-parttime-se']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/']</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>nmims mumbai mba</t>
+          <t>loans</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://sbm.nmims.edu/mba-program</t>
+          <t>https://www.tatacapital.com/personal-loan.html</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://www.nmims.edu/postgraduate-management', 'https://familybusiness.nmims.edu/postgraduate-programs/mba-real-estate-management/', 'https://sbm.nmims.edu/fulltime-programs']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/loan-restructuring-2-0-meaning-eligibility-how-to-apply/']</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>mba from narsee monjee</t>
+          <t>online loans</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://sbm.nmims.edu/mba-program</t>
+          <t>https://www.tatacapital.com/personal-loan.html</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://sbm.nmims.edu/mba-parttime-se', 'https://sbm.nmims.edu/fulltime-programs']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/']</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>mba nmims</t>
+          <t>personal loan apply online</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://sbm.nmims.edu/mba-program</t>
+          <t>https://www.tatacapital.com/personal-loan.html</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://sbm.nmims.edu/mba-parttime-se', 'https://sbm.nmims.edu/fulltime-programs']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/']</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>narsee monjee mba</t>
+          <t>instant personal loan online</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://sbm.nmims.edu/mba-program</t>
+          <t>https://www.tatacapital.com/personal-loan.html</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://sbm.nmims.edu/mba-parttime-se', 'https://sbm.nmims.edu/fulltime-programs']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/']</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>nmims mba programs</t>
+          <t>instant loan online</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://sbm.nmims.edu/mba-program</t>
+          <t>https://www.tatacapital.com/personal-loan.html</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://sbm.nmims.edu/fulltime-programs', 'https://familybusiness.nmims.edu/postgraduate-programs/mba-real-estate-management/']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/']</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>nmims mba finance</t>
+          <t>lowest interest rate personal loan</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://sbm.nmims.edu/mba-program</t>
+          <t>https://www.tatacapital.com/personal-loan.html</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://familybusiness.nmims.edu/postgraduate-programs/mba-real-estate-management/', 'https://sbm.nmims.edu/fulltime-programs']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/']</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>nmims acceptance rate</t>
+          <t>deals of loan</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://sbm.nmims.edu/mba-program</t>
+          <t>https://www.tatacapital.com/personal-loan.html</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://sbm.nmims.edu/fulltime-programs', 'https://sbm.nmims.edu/mba-parttime-se']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/', 'https://www.tatacapital.com/blog/personal-use-loan/loan-restructuring-2-0-meaning-eligibility-how-to-apply/']</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>mba in mumbai</t>
+          <t>personal loan apply</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://sbm.nmims.edu/mba-program</t>
+          <t>https://www.tatacapital.com/personal-loan.html</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://sbm.nmims.edu/fulltime-programs', 'https://sbm.nmims.edu/mba-parttime-se']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/', 'https://www.tatacapital.com/blog/personal-use-loan/loan-restructuring-2-0-meaning-eligibility-how-to-apply/']</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>nmims mba</t>
+          <t>easy loan app</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://sbm.nmims.edu/mba-program</t>
+          <t>https://www.tatacapital.com/personal-loan.html</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/fulltime-programs', 'https://sbm.nmims.edu/mba-parttime-se']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/']</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>nm college mba</t>
+          <t>low interest personal loans</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://sbm.nmims.edu/mba-program</t>
+          <t>https://www.tatacapital.com/personal-loan.html</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://sbm.nmims.edu/fulltime-programs', 'https://sbm.nmims.edu/mba-parttime-se']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/']</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>nm college mba</t>
+          <t>instant personal loan without documents</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://sbm.nmims.edu/mba-program</t>
+          <t>https://www.tatacapital.com/personal-loan.html</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://sbm.nmims.edu/fulltime-programs', 'https://sbm.nmims.edu/mba-parttime-se']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/', 'https://www.tatacapital.com/blog/personal-use-loan/loan-restructuring-2-0-meaning-eligibility-how-to-apply/']</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>nimis</t>
+          <t>small personal loans online</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://sbm.nmims.edu/mba-program</t>
+          <t>https://www.tatacapital.com/personal-loan.html</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>['https://familybusiness.nmims.edu/undergraduate-programs/integrated-mba-entrepreneurship-and-family-business/', 'https://www.nmims.edu/postgraduate-management', 'https://commerce.nmims.edu/academics-programs-bba-mba.php', 'https://sbm.nmims.edu/mba-parttime-se', 'https://familybusiness.nmims.edu/postgraduate-programs/mba-entrepreneurship/']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/']</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>nmims mba eligibility</t>
+          <t>branch personal loan app</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://sbm.nmims.edu/mba-program</t>
+          <t>https://www.tatacapital.com/personal-loan.html</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/mba-parttime-se', 'https://familybusiness.nmims.edu/postgraduate-programs/mba-real-estate-management/']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/']</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>mba from nmims</t>
+          <t>quick loans online</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>https://sbm.nmims.edu/mba-program</t>
+          <t>https://www.tatacapital.com/personal-loan.html</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://sbm.nmims.edu/mba-parttime-se', 'https://sbm.nmims.edu/fulltime-programs']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/']</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>narsee monjee mba</t>
+          <t>loan companies</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://sbm.nmims.edu/mba-program</t>
+          <t>https://www.tatacapital.com/personal-loan.html</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://sbm.nmims.edu/mba-parttime-se', 'https://sbm.nmims.edu/fulltime-programs']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/']</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>narsee monjee integrated mba</t>
+          <t>duress meaning in tamil</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://familybusiness.nmims.edu/undergraduate-programs/integrated-mba-entrepreneurship-and-family-business/</t>
+          <t>https://www.tatacapital.com/personal-loan.html</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-program', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/fulltime-programs']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/loan-restructuring-2-0-meaning-eligibility-how-to-apply/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/']</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>mba in entrepreneurship</t>
+          <t>loan app fast approval</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://familybusiness.nmims.edu/undergraduate-programs/integrated-mba-entrepreneurship-and-family-business/</t>
+          <t>https://www.tatacapital.com/personal-loan.html</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-program', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/fulltime-programs', 'https://sbm.nmims.edu/mba-executive-program.php']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/']</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>integrated mba</t>
+          <t>how to get 5 lakhs loan without interest</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>https://familybusiness.nmims.edu/undergraduate-programs/integrated-mba-entrepreneurship-and-family-business/</t>
+          <t>https://www.tatacapital.com/personal-loan.html</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-program', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/fulltime-programs', 'https://sbm.nmims.edu/mba-executive-program.php']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/']</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>nmims bba fees</t>
+          <t>tata capital helpline number</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>https://familybusiness.nmims.edu/undergraduate-programs/integrated-mba-entrepreneurship-and-family-business/</t>
+          <t>https://www.tatacapital.com/personal-loan.html</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-program', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://commerce.nmims.edu/academics-programs-bba-mba.php', 'https://familybusiness.nmims.edu/postgraduate-programs/mba-real-estate-management/']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/']</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>dalal company</t>
+          <t>personal loan for one month</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>https://familybusiness.nmims.edu/undergraduate-programs/integrated-mba-entrepreneurship-and-family-business/</t>
+          <t>https://www.tatacapital.com/personal-loan.html</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>['https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/mba-program', 'https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-parttime-se', 'https://sbm.nmims.edu/mba-executive-program.php']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/']</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>bba mba integrated</t>
+          <t>easy loan bank</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>https://familybusiness.nmims.edu/undergraduate-programs/integrated-mba-entrepreneurship-and-family-business/</t>
+          <t>https://www.tatacapital.com/personal-loan.html</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-program', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/fulltime-programs', 'https://sbm.nmims.edu/mba-executive-program.php']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/']</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>bba mba integrated course in 4 years</t>
+          <t>personal loan bad credit instant approval</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>https://familybusiness.nmims.edu/undergraduate-programs/integrated-mba-entrepreneurship-and-family-business/</t>
+          <t>https://www.tatacapital.com/personal-loan.html</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-program', 'https://www.nmims.edu/postgraduate-management', 'https://commerce.nmims.edu/academics-programs-bba-mba.php', 'https://sbm.nmims.edu/fulltime-programs']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/']</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>entrance exam for integrated mba</t>
+          <t>loans for under 21</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>https://familybusiness.nmims.edu/undergraduate-programs/integrated-mba-entrepreneurship-and-family-business/</t>
+          <t>https://www.tatacapital.com/personal-loan.html</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-program', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://sbm.nmims.edu/fulltime-programs']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/']</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>understanding business</t>
+          <t>can i get 10 lakhs personal loan</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>https://familybusiness.nmims.edu/undergraduate-programs/integrated-mba-entrepreneurship-and-family-business/</t>
+          <t>https://www.tatacapital.com/personal-loan.html</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>['https://sbm.nmims.edu/mba-program', 'https://bengaluru.nmims.edu/mba/', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/fulltime-programs', 'https://sbm.nmims.edu/mba-executive-program.php']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/']</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>bba and mba integrated course</t>
+          <t>just money loan</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>https://familybusiness.nmims.edu/undergraduate-programs/integrated-mba-entrepreneurship-and-family-business/</t>
+          <t>https://www.tatacapital.com/personal-loan.html</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-program', 'https://www.nmims.edu/postgraduate-management', 'https://commerce.nmims.edu/academics-programs-bba-mba.php', 'https://sbm.nmims.edu/mba-executive-program.php']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/']</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>efmd</t>
+          <t>loan for less interest</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>https://familybusiness.nmims.edu/undergraduate-programs/integrated-mba-entrepreneurship-and-family-business/</t>
+          <t>https://www.tatacapital.com/personal-loan.html</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>['https://www.nmims.edu/postgraduate-management', 'https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-program', 'https://sbm.nmims.edu/fulltime-programs', 'https://sbm.nmims.edu/mba-executive-program.php']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/']</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>mba in family business nmims</t>
+          <t>try my loan</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>https://familybusiness.nmims.edu/undergraduate-programs/integrated-mba-entrepreneurship-and-family-business/</t>
+          <t>https://www.tatacapital.com/personal-loan.html</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-program', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://sbm.nmims.edu/fulltime-programs']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/']</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>mba after bba</t>
+          <t>how to get personal loan with lowest interest rate</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>https://familybusiness.nmims.edu/undergraduate-programs/integrated-mba-entrepreneurship-and-family-business/</t>
+          <t>https://www.tatacapital.com/personal-loan.html</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-program', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://sbm.nmims.edu/fulltime-programs']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/']</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>mba integrated course</t>
+          <t>money loan in india</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>https://familybusiness.nmims.edu/undergraduate-programs/integrated-mba-entrepreneurship-and-family-business/</t>
+          <t>https://www.tatacapital.com/personal-loan.html</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-program', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/fulltime-programs', 'https://sbm.nmims.edu/mba-executive-program.php']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/']</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>bba and mba course</t>
+          <t>shivam cards surat</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>https://familybusiness.nmims.edu/undergraduate-programs/integrated-mba-entrepreneurship-and-family-business/</t>
+          <t>https://www.tatacapital.com/personal-loan.html</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-program', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://sbm.nmims.edu/fulltime-programs']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/']</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>integrated mba after 12th</t>
+          <t>tata capital customer care</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>https://familybusiness.nmims.edu/undergraduate-programs/integrated-mba-entrepreneurship-and-family-business/</t>
+          <t>https://www.tatacapital.com/personal-loan.html</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-program', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://commerce.nmims.edu/academics-programs-bba-mba.php']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/']</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>mukesh patel school of technology management &amp; engineering</t>
+          <t>personal loan non salaried</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>https://familybusiness.nmims.edu/undergraduate-programs/integrated-mba-entrepreneurship-and-family-business/</t>
+          <t>https://www.tatacapital.com/personal-loan.html</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-program', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/fulltime-programs', 'https://sbm.nmims.edu/mba-executive-program.php']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/loan-restructuring-2-0-meaning-eligibility-how-to-apply/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/']</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>nmims mumbai bba fees</t>
+          <t>how to personal loan</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>https://familybusiness.nmims.edu/undergraduate-programs/integrated-mba-entrepreneurship-and-family-business/</t>
+          <t>https://www.tatacapital.com/personal-loan.html</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-program', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://commerce.nmims.edu/academics-programs-bba-mba.php', 'https://familybusiness.nmims.edu/postgraduate-programs/mba-real-estate-management/']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/']</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>integrated mba means</t>
+          <t>quick personal loans</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>https://familybusiness.nmims.edu/undergraduate-programs/integrated-mba-entrepreneurship-and-family-business/</t>
+          <t>https://www.tatacapital.com/personal-loan.html</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-program', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://sbm.nmims.edu/fulltime-programs']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/']</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>nmims integrated mba</t>
+          <t>instant loan for salaried employees</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>https://familybusiness.nmims.edu/undergraduate-programs/integrated-mba-entrepreneurship-and-family-business/</t>
+          <t>https://www.tatacapital.com/personal-loan.html</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-program', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/fulltime-programs']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/', 'https://www.tatacapital.com/blog/personal-use-loan/loan-restructuring-2-0-meaning-eligibility-how-to-apply/']</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>bba mba</t>
+          <t>desired loan amount meaning</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>https://familybusiness.nmims.edu/undergraduate-programs/integrated-mba-entrepreneurship-and-family-business/</t>
+          <t>https://www.tatacapital.com/personal-loan.html</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/mba-program', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://sbm.nmims.edu/fulltime-programs']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/']</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>what is integrated mba</t>
+          <t>best personal loan interest rates</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>https://familybusiness.nmims.edu/undergraduate-programs/integrated-mba-entrepreneurship-and-family-business/</t>
+          <t>https://www.tatacapital.com/personal-loan.html</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/mba-program', 'https://sbm.nmims.edu/fulltime-programs', 'https://sbm.nmims.edu/mba-executive-program.php']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/']</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>parle company introduction</t>
+          <t>long term loan apps</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>https://familybusiness.nmims.edu/undergraduate-programs/integrated-mba-entrepreneurship-and-family-business/</t>
+          <t>https://www.tatacapital.com/personal-loan.html</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>['https://sbm.nmims.edu/mba-program', 'https://bengaluru.nmims.edu/mba/', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://sbm.nmims.edu/fulltime-programs']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/']</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>sbm nmims mumbai</t>
+          <t>1 minute loan</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>https://familybusiness.nmims.edu/undergraduate-programs/integrated-mba-entrepreneurship-and-family-business/</t>
+          <t>https://www.tatacapital.com/personal-loan.html</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-program', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://sbm.nmims.edu/mba-parttime-se']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/']</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>narsee monjee vile parle</t>
+          <t>easy to get personal loans</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>https://familybusiness.nmims.edu/undergraduate-programs/integrated-mba-entrepreneurship-and-family-business/</t>
+          <t>https://www.tatacapital.com/personal-loan.html</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-program', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://sbm.nmims.edu/mba-parttime-se']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/']</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>live projects for mba</t>
+          <t>online personal loan bank</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>https://familybusiness.nmims.edu/undergraduate-programs/integrated-mba-entrepreneurship-and-family-business/</t>
+          <t>https://www.tatacapital.com/personal-loan.html</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-program', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/fulltime-programs', 'https://sbm.nmims.edu/mba-executive-program.php']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/']</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>family business management course</t>
+          <t>crif cibil login</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>https://familybusiness.nmims.edu/undergraduate-programs/integrated-mba-entrepreneurship-and-family-business/</t>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>['https://sbm.nmims.edu/mba-program', 'https://bengaluru.nmims.edu/mba/', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/fulltime-programs', 'https://sbm.nmims.edu/mba-executive-program.php']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/personal-loan.html', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/']</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>narsee monjee bba fees</t>
+          <t>commercial crif</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>https://familybusiness.nmims.edu/undergraduate-programs/integrated-mba-entrepreneurship-and-family-business/</t>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-program', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://commerce.nmims.edu/academics-programs-bba-mba.php', 'https://www.nmims.edu/postgraduate-management']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/personal-loan.html']</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>nmims post graduate courses</t>
+          <t>commercial crif</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>https://sbm.nmims.edu/fulltime-programs</t>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-program', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://sbm.nmims.edu/mba-parttime-se']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/personal-loan.html']</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>narsee monjee courses</t>
+          <t>full form of cri</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>https://sbm.nmims.edu/fulltime-programs</t>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-program', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://sbm.nmims.edu/mba-parttime-se']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/personal-loan.html']</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>nmims mba programs</t>
+          <t>highmark credit score</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>https://sbm.nmims.edu/fulltime-programs</t>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-program', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://familybusiness.nmims.edu/postgraduate-programs/mba-real-estate-management/']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/']</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>nmims mba</t>
+          <t>crif credit report means</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>https://sbm.nmims.edu/fulltime-programs</t>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-program', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/mba-parttime-se']</t>
+          <t>['https://www.tatacapital.com/personal-loan.html', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/']</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>nmims courses</t>
+          <t>check crif score</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>https://sbm.nmims.edu/fulltime-programs</t>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-program', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://sbm.nmims.edu/mba-parttime-se']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/']</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>nmims healthcare management</t>
+          <t>crif consumer</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>https://sbm.nmims.edu/fulltime-programs</t>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-program', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://sbm.nmims.edu/mba-parttime-se']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/', 'https://www.tatacapital.com/personal-loan.html', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/']</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>nmims mba fees for 2 years</t>
+          <t>what is crif score</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>https://sbm.nmims.edu/fulltime-programs</t>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-program', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://www.nmims.edu/postgraduate-management', 'https://commerce.nmims.edu/academics-programs-bba-mba.php']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/']</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>nmims pg courses</t>
+          <t>crif member login</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>https://sbm.nmims.edu/fulltime-programs</t>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-program', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://sbm.nmims.edu/mba-parttime-se']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/personal-loan.html', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/']</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>nmims pharma mba</t>
+          <t>eligibility certificate meaning in marathi</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>https://sbm.nmims.edu/fulltime-programs</t>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-program', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://familybusiness.nmims.edu/postgraduate-programs/mba-real-estate-management/']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/', 'https://www.tatacapital.com/blog/personal-use-loan/loan-restructuring-2-0-meaning-eligibility-how-to-apply/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/']</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>mba from nmims</t>
+          <t>crif score vs cibil score</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>https://sbm.nmims.edu/fulltime-programs</t>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-program', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://sbm.nmims.edu/mba-parttime-se']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/']</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>nmims courses offered</t>
+          <t>highmark score</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>https://sbm.nmims.edu/fulltime-programs</t>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-program', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://sbm.nmims.edu/mba-parttime-se']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/', 'https://www.tatacapital.com/personal-loan.html']</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>nmims pgdm</t>
+          <t>crif score meaning</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>https://sbm.nmims.edu/fulltime-programs</t>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-program', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://familybusiness.nmims.edu/postgraduate-programs/mba-real-estate-management/']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/']</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>mba courses</t>
+          <t>du cutoff list 2022</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>https://sbm.nmims.edu/fulltime-programs</t>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-program', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://familybusiness.nmims.edu/postgraduate-programs/mba-real-estate-management/']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/loan-restructuring-2-0-meaning-eligibility-how-to-apply/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/']</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>mba from narsee monjee</t>
+          <t>crif meaning</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>https://sbm.nmims.edu/fulltime-programs</t>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-program', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://sbm.nmims.edu/mba-parttime-se']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/', 'https://www.tatacapital.com/personal-loan.html', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/']</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>nmims part time mba</t>
+          <t>crif customer care number</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>https://sbm.nmims.edu/fulltime-programs</t>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-program', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://sbm.nmims.edu/mba-parttime-se']</t>
+          <t>['https://www.tatacapital.com/personal-loan.html', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/']</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>nmims mba courses</t>
+          <t>crif score check</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>https://sbm.nmims.edu/fulltime-programs</t>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-program', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://familybusiness.nmims.edu/postgraduate-programs/mba-real-estate-management/']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/']</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>nmims mumbai mba</t>
+          <t>crif highmark customer care number</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>https://sbm.nmims.edu/fulltime-programs</t>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-program', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://www.nmims.edu/postgraduate-management', 'https://familybusiness.nmims.edu/postgraduate-programs/mba-real-estate-management/']</t>
+          <t>['https://www.tatacapital.com/personal-loan.html', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/']</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>mba domains</t>
+          <t>how to increase crif score</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>https://sbm.nmims.edu/fulltime-programs</t>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>['https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/mba-program', 'https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://sbm.nmims.edu/mba-parttime-se']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/']</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>nmims part time mba fees</t>
+          <t>crif cibil report</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>https://sbm.nmims.edu/fulltime-programs</t>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-program', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/mba-parttime-se']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/']</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>mba nmims</t>
+          <t>crif full form</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>https://sbm.nmims.edu/fulltime-programs</t>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/mba-program', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://sbm.nmims.edu/mba-parttime-se']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/']</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>narsee monjee mba</t>
+          <t>crif vs cibil</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>https://sbm.nmims.edu/fulltime-programs</t>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-program', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://sbm.nmims.edu/mba-parttime-se']</t>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/']</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>nmims mumbai courses</t>
+          <t>pf amount check online</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>https://sbm.nmims.edu/fulltime-programs</t>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>['https://bengaluru.nmims.edu/mba/', 'https://sbm.nmims.edu/mba-program', 'https://www.nmims.edu/postgraduate-management', 'https://sbm.nmims.edu/mba-executive-program.php', 'https://sbm.nmims.edu/mba-parttime-se']</t>
+          <t>['https://www.tatacapital.com/personal-loan.html', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/']</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>check passbook</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/personal-loan.html', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/']</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>epfo know balance</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/']</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>una active online</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>['https://www.tatacapital.com/personal-loan.html', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/']</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>epf ppo enquiry</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/', 'https://www.tatacapital.com/blog/personal-use-loan/loan-restructuring-2-0-meaning-eligibility-how-to-apply/']</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>http epfigms gov in</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>['https://www.tatacapital.com/personal-loan.html', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/']</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>home member portal</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>['https://www.tatacapital.com/personal-loan.html', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/', 'https://www.tatacapital.com/blog/personal-use-loan/loan-restructuring-2-0-meaning-eligibility-how-to-apply/']</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>what is mean by pf</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>['https://www.tatacapital.com/personal-loan.html', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/loan-restructuring-2-0-meaning-eligibility-how-to-apply/']</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>pdf pf</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>['https://www.tatacapital.com/personal-loan.html', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/', 'https://www.tatacapital.com/blog/personal-use-loan/loan-restructuring-2-0-meaning-eligibility-how-to-apply/', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/']</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>www epf com login</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/personal-loan.html', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/']</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>uan login pf balance check</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/']</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>how to know pf balance with uan</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/personal-loan.html', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/']</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>epf passbook registration</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/personal-loan.html', 'https://www.tatacapital.com/blog/personal-use-loan/loan-restructuring-2-0-meaning-eligibility-how-to-apply/']</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>pf office rohtak</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>['https://www.tatacapital.com/personal-loan.html', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/']</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>check member pf balance</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/', 'https://www.tatacapital.com/personal-loan.html', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/']</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>pf check contact number</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>['https://www.tatacapital.com/personal-loan.html', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/']</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>member passbook pf</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/', 'https://www.tatacapital.com/blog/personal-use-loan/loan-restructuring-2-0-meaning-eligibility-how-to-apply/']</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>www member passbook</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>['https://www.tatacapital.com/personal-loan.html', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/']</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>how to check pf amount online</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/']</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>www epfindia gov in passbook</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/', 'https://www.tatacapital.com/blog/personal-use-loan/loan-restructuring-2-0-meaning-eligibility-how-to-apply/']</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>how to open epf passbook</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/personal-loan.html', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/']</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>epfo balance enquiry number</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>['https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/', 'https://www.tatacapital.com/blog/personal-use-loan/800-plus-credit-score-how-to-make-the-most-of-it/', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/personal-loan.html', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/']</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>pf online member login</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>https://www.tatacapital.com/blog/personal-use-loan/how-to-check-pf-balance-online/</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>['https://www.tatacapital.com/personal-loan.html', 'https://www.tatacapital.com/blog/personal-use-loan/crif-highmark-score-meaning-full-form-and-how-to-apply/', 'https://www.tatacapital.com/blog/personal-use-loan/payday-loans-in-india-what-is-a-payday-loan-and-how-does-it-work-in-india/', 'https://www.tatacapital.com/blog/personal-use-loan/how-to-get-a-10000-loan-on-aadhar-card/', 'https://www.tatacapital.com/blog/personal-use-loan/difference-between-rupay-and-visa-card/']</t>
         </is>
       </c>
     </row>

</xml_diff>